<commit_message>
add note on 010820 sim results
</commit_message>
<xml_diff>
--- a/Simulation Results 010820.xlsx
+++ b/Simulation Results 010820.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrianLam/UTSC Research/Plaut_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25F724B6-7867-134A-A6E8-E455E7158B22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEDDB4F-401E-3841-B7C5-C1B319AB2D89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{731A8A60-4D85-694D-9B57-3EC626427640}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" activeTab="2" xr2:uid="{731A8A60-4D85-694D-9B57-3EC626427640}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
   <si>
     <t>Simulation 1</t>
   </si>
@@ -88,12 +88,15 @@
   <si>
     <t>Anchor 1, 2, and 3</t>
   </si>
+  <si>
+    <t>NOTE: THIS IS BEFORE THE UPDATE ON JAN 8, 2020 ON HOW LOSS IS CALCULATED</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,13 +119,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,10 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1394,15 +1414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD921E4F-5EDE-5B4E-8C59-9131F66B71AC}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I1" sqref="I1:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1411,8 +1431,16 @@
       <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1421,8 +1449,14 @@
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1431,8 +1465,14 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1441,8 +1481,14 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1451,8 +1497,14 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1461,8 +1513,14 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1471,8 +1529,17 @@
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:N7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1480,15 +1547,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91334DBB-3320-CA41-8063-97F176F4831A}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I1" sqref="I1:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1497,8 +1564,16 @@
       <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1507,8 +1582,14 @@
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1517,8 +1598,14 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1527,8 +1614,14 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1537,8 +1630,14 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1547,8 +1646,14 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1557,8 +1662,17 @@
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:N7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1566,15 +1680,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A30168-F67C-BC4E-A581-6173ACDBEC56}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="41" workbookViewId="0">
-      <selection activeCell="O55" sqref="O55"/>
+      <selection activeCell="I1" sqref="I1:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1583,8 +1697,16 @@
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1593,8 +1715,14 @@
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1603,8 +1731,14 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1613,8 +1747,14 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1623,8 +1763,14 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1633,8 +1779,14 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1643,8 +1795,17 @@
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:N7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update code and 011220 reults
</commit_message>
<xml_diff>
--- a/Simulation Results 010820.xlsx
+++ b/Simulation Results 010820.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrianLam/UTSC Research/Plaut_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEDDB4F-401E-3841-B7C5-C1B319AB2D89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC975177-2C80-DF40-ACF3-CA6F43D8298C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" activeTab="2" xr2:uid="{731A8A60-4D85-694D-9B57-3EC626427640}"/>
   </bookViews>
   <sheets>
-    <sheet name="Simulation 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Simulation 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Simulation 3" sheetId="3" r:id="rId3"/>
+    <sheet name="N" sheetId="1" r:id="rId1"/>
+    <sheet name="2N" sheetId="2" r:id="rId2"/>
+    <sheet name="3N" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1683,7 +1683,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="41" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:N7"/>
+      <selection activeCell="R49" sqref="R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>